<commit_message>
Ouais j'ai fait plein de trucs t'as vu
J'aurais dû prendre le temps de détailler plusieurs commits
</commit_message>
<xml_diff>
--- a/Messages.xlsx
+++ b/Messages.xlsx
@@ -136,15 +136,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -346,11 +352,143 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -376,6 +514,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -391,56 +535,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF7C9B3F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF7C9B3F"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF7C9B3F"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <b val="0"/>
@@ -455,58 +590,15 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF7C9B3F"/>
+      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00863D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF7C9B3F"/>
         </patternFill>
       </fill>
     </dxf>
@@ -808,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -819,18 +911,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1">
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
@@ -856,7 +948,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="b">
@@ -885,7 +977,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="b">
@@ -914,7 +1006,7 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="b">
@@ -943,7 +1035,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="b">
@@ -972,7 +1064,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="b">
@@ -1001,7 +1093,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2" t="b">
@@ -1030,7 +1122,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="2" t="b">
@@ -1059,7 +1151,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="2" t="b">
@@ -1088,7 +1180,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2" t="b">
@@ -1117,7 +1209,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="2" t="b">
@@ -1146,7 +1238,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="2" t="b">
@@ -1175,7 +1267,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="2" t="b">
@@ -1204,7 +1296,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="2" t="b">
@@ -1233,7 +1325,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="2" t="b">
@@ -1262,7 +1354,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="2" t="b">
@@ -1291,7 +1383,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="2" t="b">
@@ -1319,11 +1411,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:7" ht="15" thickBot="1">
+      <c r="A19" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="2" t="b">
+      <c r="B19" s="18" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
@@ -1343,20 +1435,20 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="G19" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="14" t="s">
+      <c r="G19" s="24" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1">
+      <c r="A20" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="2" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="C20" s="2" t="b">
+      <c r="B20" s="20" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C20" s="17" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
@@ -1368,24 +1460,24 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="F20" s="2" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="G20" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="14" t="s">
+      <c r="F20" s="23" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="20" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" thickBot="1">
+      <c r="A21" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="2" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="C21" s="2" t="b">
+      <c r="B21" s="20" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C21" s="17" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
@@ -1397,20 +1489,20 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="F21" s="2" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="G21" s="6" t="b">
+      <c r="F21" s="23" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="22" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="2" t="b">
+      <c r="B22" s="19" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
@@ -1430,13 +1522,13 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="G22" s="6" t="b">
+      <c r="G22" s="25" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="2" t="b">
@@ -1464,11 +1556,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="14" t="s">
+    <row r="24" spans="1:7" ht="15" thickBot="1">
+      <c r="A24" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="2" t="b">
+      <c r="B24" s="18" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
@@ -1488,20 +1580,20 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="G24" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="14" t="s">
+      <c r="G24" s="24" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" thickBot="1">
+      <c r="A25" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="2" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="C25" s="2" t="b">
+      <c r="B25" s="21" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C25" s="17" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
@@ -1513,24 +1605,24 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="F25" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G25" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="14" t="s">
+      <c r="F25" s="23" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="26" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" thickBot="1">
+      <c r="A26" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="2" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="C26" s="2" t="b">
+      <c r="B26" s="21" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C26" s="17" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
@@ -1542,24 +1634,24 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="F26" s="2" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="G26" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="14" t="s">
+      <c r="F26" s="23" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="G26" s="20" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" thickBot="1">
+      <c r="A27" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="2" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="C27" s="2" t="b">
+      <c r="B27" s="21" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C27" s="17" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
@@ -1571,24 +1663,24 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="F27" s="2" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="G27" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="14" t="s">
+      <c r="F27" s="23" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="G27" s="20" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" thickBot="1">
+      <c r="A28" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="2" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="C28" s="2" t="b">
+      <c r="B28" s="21" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C28" s="17" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
@@ -1600,24 +1692,24 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="F28" s="2" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="G28" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="14" t="s">
+      <c r="F28" s="23" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="G28" s="27" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" thickBot="1">
+      <c r="A29" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="2" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="C29" s="2" t="b">
+      <c r="B29" s="22" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C29" s="17" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
@@ -1629,20 +1721,20 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="F29" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G29" s="6" t="b">
+      <c r="F29" s="23" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="22" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="2" t="b">
+      <c r="B30" s="19" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
@@ -1662,13 +1754,13 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="G30" s="6" t="b">
+      <c r="G30" s="25" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15" thickBot="1">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B31" s="7" t="b">
@@ -1703,10 +1795,10 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:G31">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>B3=TRUE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>B3=FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>